<commit_message>
Replace data in template with empty or placeholder
</commit_message>
<xml_diff>
--- a/Konsulttidrapport.xlsx
+++ b/Konsulttidrapport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.nilefalk\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.nilefalk\Utveckling\td2tlu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48DBF7A-7BDE-4122-8A5F-9E30578787F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEE620-40FE-44AC-AF50-43B41BAFB3B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9720" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Januari 2019" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -103,22 +105,22 @@
     <t>Övrigt Projektnr</t>
   </si>
   <si>
-    <t>11402-12</t>
-  </si>
-  <si>
-    <t>Thomas Nilefalk</t>
-  </si>
-  <si>
     <t>Responsive AB</t>
   </si>
   <si>
-    <t>Februari 2020</t>
-  </si>
-  <si>
-    <t>Java SDK</t>
-  </si>
-  <si>
     <t>Mats Bengtsson</t>
+  </si>
+  <si>
+    <t>&lt;user&gt;</t>
+  </si>
+  <si>
+    <t>&lt;projno&gt;</t>
+  </si>
+  <si>
+    <t>&lt;month&gt;</t>
+  </si>
+  <si>
+    <t>&lt;team&gt;</t>
   </si>
 </sst>
 </file>
@@ -536,8 +538,8 @@
   </sheetPr>
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -597,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -618,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -639,7 +641,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -660,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -681,7 +683,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -841,9 +843,7 @@
       <c r="A14" s="5">
         <v>43868</v>
       </c>
-      <c r="B14" s="6">
-        <v>5</v>
-      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -858,7 +858,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1020,9 +1020,7 @@
       <c r="A22" s="5">
         <v>43876</v>
       </c>
-      <c r="B22" s="6">
-        <v>6</v>
-      </c>
+      <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1037,7 +1035,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="12"/>
     </row>
@@ -1156,9 +1154,7 @@
       <c r="A28" s="5">
         <v>43882</v>
       </c>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
+      <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1173,7 +1169,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -1401,7 +1397,8 @@
         <v>11</v>
       </c>
       <c r="B39" s="11">
-        <v>12</v>
+        <f>SUM(B8:B38)</f>
+        <v>0</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -1436,7 +1433,7 @@
       <c r="N40" s="2"/>
       <c r="O40" s="7">
         <f>SUM(O8:O38)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename tab to not say month
</commit_message>
<xml_diff>
--- a/Konsulttidrapport.xlsx
+++ b/Konsulttidrapport.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.nilefalk\Utveckling\td2tlu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEE620-40FE-44AC-AF50-43B41BAFB3B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2CA46A-AB22-4DDC-8ACA-51725B3867BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9720" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Januari 2019" sheetId="1" r:id="rId1"/>
+    <sheet name="Konsulttidrapport" sheetId="1" r:id="rId1"/>
     <sheet name="Beskrivning till mallen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -223,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -245,6 +245,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,7 +540,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,43 +556,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -619,63 +620,63 @@
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -711,7 +712,7 @@
       <c r="A8" s="5">
         <v>43862</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -733,7 +734,7 @@
       <c r="A9" s="5">
         <v>43863</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -755,7 +756,7 @@
       <c r="A10" s="5">
         <v>43864</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -777,7 +778,7 @@
       <c r="A11" s="5">
         <v>43865</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -799,7 +800,7 @@
       <c r="A12" s="5">
         <v>43866</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -821,7 +822,7 @@
       <c r="A13" s="5">
         <v>43867</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -843,7 +844,7 @@
       <c r="A14" s="5">
         <v>43868</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -865,7 +866,7 @@
       <c r="A15" s="5">
         <v>43869</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -887,7 +888,7 @@
       <c r="A16" s="5">
         <v>43870</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -909,7 +910,7 @@
       <c r="A17" s="5">
         <v>43871</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -931,7 +932,7 @@
       <c r="A18" s="5">
         <v>43872</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -953,7 +954,7 @@
       <c r="A19" s="5">
         <v>43873</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -975,7 +976,7 @@
       <c r="A20" s="5">
         <v>43874</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -997,7 +998,7 @@
       <c r="A21" s="5">
         <v>43875</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1020,7 +1021,7 @@
       <c r="A22" s="5">
         <v>43876</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1043,7 +1044,7 @@
       <c r="A23" s="5">
         <v>43877</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1066,7 +1067,7 @@
       <c r="A24" s="5">
         <v>43878</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1088,7 +1089,7 @@
       <c r="A25" s="5">
         <v>43879</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1110,7 +1111,7 @@
       <c r="A26" s="5">
         <v>43880</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1132,7 +1133,7 @@
       <c r="A27" s="5">
         <v>43881</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1154,7 +1155,7 @@
       <c r="A28" s="5">
         <v>43882</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1176,7 +1177,7 @@
       <c r="A29" s="5">
         <v>43883</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1198,7 +1199,7 @@
       <c r="A30" s="5">
         <v>43884</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1220,7 +1221,7 @@
       <c r="A31" s="5">
         <v>43885</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1242,7 +1243,7 @@
       <c r="A32" s="5">
         <v>43886</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1264,7 +1265,7 @@
       <c r="A33" s="5">
         <v>43887</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1286,7 +1287,7 @@
       <c r="A34" s="5">
         <v>43888</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1308,7 +1309,7 @@
       <c r="A35" s="5">
         <v>43889</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1330,7 +1331,7 @@
       <c r="A36" s="5">
         <v>43890</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1352,7 +1353,7 @@
       <c r="A37" s="5">
         <v>43891</v>
       </c>
-      <c r="B37" s="6"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1374,7 +1375,7 @@
       <c r="A38" s="5">
         <v>43892</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>

</xml_diff>